<commit_message>
More comprehensive excel and csv import, bringing in limits as part of the headers.
</commit_message>
<xml_diff>
--- a/examples/example_data.xlsx
+++ b/examples/example_data.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
+    <t xml:space="preserve">value (lsl=-2.5 usl=2.5)</t>
   </si>
 </sst>
 </file>
@@ -40,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -124,10 +125,10 @@
   <dimension ref="A4:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>

</xml_diff>

<commit_message>
Adding starting control plot.
</commit_message>
<xml_diff>
--- a/examples/example_data.xlsx
+++ b/examples/example_data.xlsx
@@ -125,13 +125,13 @@
   <dimension ref="A4:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,7 +235,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2.18235828</v>
+        <v>-2.51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Better control chart with more samples.
</commit_message>
<xml_diff>
--- a/examples/example_data.xlsx
+++ b/examples/example_data.xlsx
@@ -125,10 +125,10 @@
   <dimension ref="A4:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>
@@ -235,7 +235,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-2.51</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Major refactor to make the API more consistent with community standards for plotting along with manufacturing terminology.
</commit_message>
<xml_diff>
--- a/examples/example_data.xlsx
+++ b/examples/example_data.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">value (lsl=-2.5 usl=2.5)</t>
+    <t xml:space="preserve">value (lcl=-2.5 ucl=2.5)</t>
   </si>
 </sst>
 </file>
@@ -125,10 +125,10 @@
   <dimension ref="A4:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>

</xml_diff>